<commit_message>
changing the sample files
</commit_message>
<xml_diff>
--- a/data/sample.xlsx
+++ b/data/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardamri/Desktop/Files/לימודים/תואר שני/קורסי קדם/למידה חישובית - 37225214/RAG_System/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardamri/Desktop/RAG_System/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D029465-A203-AD4B-8C48-42CF03582338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C863F4-84A4-E84C-9CD3-4483DC666005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="860" windowWidth="28040" windowHeight="16940" xr2:uid="{7E5EE352-61C8-A148-9457-A71FF4B5511E}"/>
+    <workbookView xWindow="540" yWindow="780" windowWidth="28040" windowHeight="16940" xr2:uid="{7E5EE352-61C8-A148-9457-A71FF4B5511E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,37 +36,103 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Data scientist working on RAG</t>
-  </si>
-  <si>
-    <t>Bar</t>
-  </si>
-  <si>
-    <t>Charlie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software engineer at Microsoft </t>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Role Description</t>
+  </si>
+  <si>
+    <t>Bar Damri</t>
+  </si>
+  <si>
+    <t>CEO &amp; Head of AI</t>
+  </si>
+  <si>
+    <t>Management / Technology</t>
+  </si>
+  <si>
+    <t>Founder of QuantumFlow AI, he manages technological development and research in artificial intelligence.</t>
+  </si>
+  <si>
+    <t>Tali Cohen</t>
+  </si>
+  <si>
+    <t>Senior Project Manager</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Responsible for managing custom development projects, including client communication and scheduling.</t>
+  </si>
+  <si>
+    <t>Yoav Levi</t>
+  </si>
+  <si>
+    <t>Software Architect</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Designs the microservices architecture and oversees the implementation of cloud solutions.</t>
+  </si>
+  <si>
+    <t>Rotem Sharabi</t>
+  </si>
+  <si>
+    <t>Fullstack Developer</t>
+  </si>
+  <si>
+    <t>Develops the client-side (React) and server-side (FastAPI) of the company's applications.</t>
+  </si>
+  <si>
+    <t>Gil Yitzhak</t>
+  </si>
+  <si>
+    <t>Data Scientist</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>Analyzes the performance of AI models and develops new algorithms to improve RAG systems.</t>
+  </si>
+  <si>
+    <t>Anna Pollak</t>
+  </si>
+  <si>
+    <t>Backend Developer</t>
+  </si>
+  <si>
+    <t>Responsible for developing and implementing databases (MongoDB, Redis) and improving server performance.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,8 +155,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,40 +492,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24E92E1-2591-7247-937A-C5534C5AF7CC}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>